<commit_message>
consistent naming histtag vs hist_tag
</commit_message>
<xml_diff>
--- a/data/input/consistency_input.xlsx
+++ b/data/input/consistency_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="inhoudsopgave" sheetId="1" state="visible" r:id="rId2"/>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">hisTags die niet konden worden gemapped naar interne locatie en niet in de hisTag_ignore zijn opgenomen</t>
   </si>
   <si>
-    <t xml:space="preserve">histTags ignore match</t>
+    <t xml:space="preserve">ignored histTags match</t>
   </si>
   <si>
     <t xml:space="preserve">hisTags uit de histTag_ignore die wél in de idmaps zijn opgenomen</t>
@@ -2205,19 +2205,19 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="120.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="120.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
@@ -2510,14 +2510,15 @@
   </sheetPr>
   <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5702,7 +5703,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
@@ -5788,7 +5789,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
@@ -5858,7 +5859,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>

</xml_diff>